<commit_message>
Add XBB Comparison Results
</commit_message>
<xml_diff>
--- a/subvariants/XBB.1_recombination/HADDOCK_Results.xlsx
+++ b/subvariants/XBB.1_recombination/HADDOCK_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Documents\GitHub\SARS-CoV-2_B.1.1.529_Spike-RBD_Predictions\subvariants\XBB.1_recombination\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD8724B-1D1C-46E9-96AD-377EB9069E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3A1907-7D0B-4A63-BDDC-A04603765F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{62A41C40-034E-4CCB-9F98-C69E7335804C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="45">
   <si>
     <t>Antibody Name</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>7mmo_chainsHL_renumberedLplus1000 _fixed.pdb</t>
+  </si>
+  <si>
+    <t>.323.4</t>
   </si>
 </sst>
 </file>
@@ -242,12 +245,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="45"/>
     </xf>
@@ -260,20 +263,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,7 +589,10 @@
   <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,18 +729,66 @@
         <f>_xlfn.CONCAT(SUBSTITUTE(D2,".","_"),"__",A2)</f>
         <v>BJ_1__LY-CoV1404</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="K2" s="1">
+        <v>-115.4</v>
+      </c>
+      <c r="L2" s="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="M2" s="1">
+        <v>11</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="P2" s="1">
+        <v>-94.7</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="R2" s="1">
+        <v>-167.3</v>
+      </c>
+      <c r="S2" s="1">
+        <v>14.6</v>
+      </c>
+      <c r="T2" s="1">
+        <v>-33</v>
+      </c>
+      <c r="U2" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="V2" s="1">
+        <v>457.8</v>
+      </c>
+      <c r="W2" s="1">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="X2" s="1">
+        <v>2612</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>51.2</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>-2.1</v>
+      </c>
     </row>
     <row r="3" spans="1:26" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -762,16 +810,64 @@
         <f>_xlfn.CONCAT(SUBSTITUTE(D3,".","_"),"__",A3)</f>
         <v>BJ_1__AZD1061</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="10"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="K3" s="1">
+        <v>-86.3</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="M3" s="1">
+        <v>29</v>
+      </c>
+      <c r="N3" s="1">
+        <v>17.7</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="P3" s="1">
+        <v>-66.599999999999994</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="R3" s="1">
+        <v>-321.5</v>
+      </c>
+      <c r="S3" s="1">
+        <v>31.4</v>
+      </c>
+      <c r="T3" s="1">
+        <v>-9.1999999999999993</v>
+      </c>
+      <c r="U3" s="1">
+        <v>5.9</v>
+      </c>
+      <c r="V3" s="1">
+        <v>538.29999999999995</v>
+      </c>
+      <c r="W3" s="1">
+        <v>55.5</v>
+      </c>
+      <c r="X3" s="1">
+        <v>2445.9</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>77.7</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>-1.7</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -793,12 +889,60 @@
         <f t="shared" ref="G4:G10" si="0">_xlfn.CONCAT(SUBSTITUTE(D4,".","_"),"__",A4)</f>
         <v>BJ_1__AZD8895</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="9"/>
       <c r="J4" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>-111.8</v>
+      </c>
+      <c r="L4" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="M4" s="1">
+        <v>9</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="P4" s="1">
+        <v>-80.900000000000006</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="R4" s="1">
+        <v>-259.5</v>
+      </c>
+      <c r="S4" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="T4" s="1">
+        <v>-8.5</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="V4" s="1">
+        <v>294.39999999999998</v>
+      </c>
+      <c r="W4" s="1">
+        <v>46</v>
+      </c>
+      <c r="X4" s="1">
+        <v>2536.5</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>195.9</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>-2.4</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="45" x14ac:dyDescent="0.25">
@@ -824,16 +968,64 @@
         <f t="shared" si="0"/>
         <v>BM_1_1_1__LY-CoV1404</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="9"/>
       <c r="J5" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="K5" s="1">
+        <v>-103</v>
+      </c>
+      <c r="L5" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="M5" s="1">
+        <v>38</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="P5" s="1">
+        <v>-75.5</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="R5" s="1">
+        <v>-275.5</v>
+      </c>
+      <c r="S5" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="T5" s="1">
+        <v>-9.9</v>
+      </c>
+      <c r="U5" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="V5" s="1">
+        <v>375.3</v>
+      </c>
+      <c r="W5" s="1">
+        <v>34.5</v>
+      </c>
+      <c r="X5" s="1">
+        <v>2110.8000000000002</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>36</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>-1.6</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -855,16 +1047,64 @@
         <f t="shared" si="0"/>
         <v>BM_1_1_1__AZD1061</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="9"/>
       <c r="J6" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="K6" s="1">
+        <v>-102.8</v>
+      </c>
+      <c r="L6" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="M6" s="1">
+        <v>119</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="P6" s="1">
+        <v>-80.099999999999994</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>7</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S6" s="1">
+        <v>45</v>
+      </c>
+      <c r="T6" s="1">
+        <v>-6.8</v>
+      </c>
+      <c r="U6" s="1">
+        <v>1</v>
+      </c>
+      <c r="V6" s="1">
+        <v>487.2</v>
+      </c>
+      <c r="W6" s="1">
+        <v>82.7</v>
+      </c>
+      <c r="X6" s="1">
+        <v>2555.6999999999998</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>-2.1</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -886,12 +1126,60 @@
         <f t="shared" si="0"/>
         <v>BM_1_1_1__AZD8895</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="10"/>
+      <c r="I7" s="9"/>
       <c r="J7" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K7" s="1">
+        <v>-100.2</v>
+      </c>
+      <c r="L7" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="M7" s="1">
+        <v>21</v>
+      </c>
+      <c r="N7" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="P7" s="1">
+        <v>-76.400000000000006</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="R7" s="1">
+        <v>-283.39999999999998</v>
+      </c>
+      <c r="S7" s="1">
+        <v>37.6</v>
+      </c>
+      <c r="T7" s="1">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="U7" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="V7" s="1">
+        <v>231.9</v>
+      </c>
+      <c r="W7" s="1">
+        <v>31.5</v>
+      </c>
+      <c r="X7" s="1">
+        <v>2413.3000000000002</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>56</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>-1.9</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="45" x14ac:dyDescent="0.25">
@@ -917,12 +1205,60 @@
         <f t="shared" si="0"/>
         <v>XBB_1_5__LY-CoV1404</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="10"/>
+      <c r="I8" s="9"/>
       <c r="J8" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K8" s="1">
+        <v>-112.2</v>
+      </c>
+      <c r="L8" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="M8" s="1">
+        <v>96</v>
+      </c>
+      <c r="N8" s="1">
+        <v>13.1</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="P8" s="1">
+        <v>-60</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="R8" s="1">
+        <v>-396.2</v>
+      </c>
+      <c r="S8" s="1">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="T8" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="U8" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="V8" s="1">
+        <v>255</v>
+      </c>
+      <c r="W8" s="1">
+        <v>52.3</v>
+      </c>
+      <c r="X8" s="1">
+        <v>2451.1999999999998</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>164.8</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>-1.1000000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="60" x14ac:dyDescent="0.25">
@@ -948,16 +1284,64 @@
         <f t="shared" si="0"/>
         <v>XBB_1_5__AZD1061</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="10"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="K9" s="1">
+        <v>-101.4</v>
+      </c>
+      <c r="L9" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M9" s="1">
+        <v>35</v>
+      </c>
+      <c r="N9" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="O9" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="P9" s="1">
+        <v>-82.6</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="R9" s="1">
+        <v>-246.6</v>
+      </c>
+      <c r="S9" s="1">
+        <v>57</v>
+      </c>
+      <c r="T9" s="1">
+        <v>-7.9</v>
+      </c>
+      <c r="U9" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="V9" s="1">
+        <v>384.3</v>
+      </c>
+      <c r="W9" s="1">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="X9" s="1">
+        <v>2464.5</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>87.4</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>-1.1000000000000001</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -979,12 +1363,60 @@
         <f t="shared" si="0"/>
         <v>XBB_1_5__AZD8895</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="10"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="K10" s="1">
+        <v>-99.6</v>
+      </c>
+      <c r="L10" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="M10" s="1">
+        <v>62</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="P10" s="1">
+        <v>-71.8</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>12.7</v>
+      </c>
+      <c r="R10" s="1">
+        <v>-290.3</v>
+      </c>
+      <c r="S10" s="1">
+        <v>26.3</v>
+      </c>
+      <c r="T10" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="U10" s="1">
+        <v>5.9</v>
+      </c>
+      <c r="V10" s="1">
+        <v>217.7</v>
+      </c>
+      <c r="W10" s="1">
+        <v>26</v>
+      </c>
+      <c r="X10" s="1">
+        <v>2319.5</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>115.4</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>-1.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add XBB.1.5 DJM files
</commit_message>
<xml_diff>
--- a/subvariants/XBB.1_recombination/HADDOCK_Results.xlsx
+++ b/subvariants/XBB.1_recombination/HADDOCK_Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Documents\GitHub\SARS-CoV-2_B.1.1.529_Spike-RBD_Predictions\subvariants\XBB.1_recombination\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colby/SARS-CoV-2_B.1.1.529_Spike-RBD_Predictions/subvariants/XBB.1_recombination/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A3415F-336F-4F68-B8CF-92CA015E30AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58665C58-F13C-D84B-A15E-B085B7D3EB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{62A41C40-034E-4CCB-9F98-C69E7335804C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20100" xr2:uid="{62A41C40-034E-4CCB-9F98-C69E7335804C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="51">
   <si>
     <t>Antibody Name</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>Cluster 2</t>
+  </si>
+  <si>
+    <t>XBB.1.5_DJM</t>
+  </si>
+  <si>
+    <t>XBB_1_5_DJM_ff8e4_relaxed_rank_1_model_1_renumbered.pdb</t>
   </si>
 </sst>
 </file>
@@ -281,11 +287,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -601,48 +607,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A0155A-1E79-46A6-BA76-B5BBE5928165}">
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="71.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="36.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="36.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="1"/>
+    <col min="19" max="19" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="184.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="182" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -673,7 +679,7 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>45</v>
       </c>
       <c r="L1" s="3" t="s">
@@ -725,7 +731,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
@@ -751,7 +757,7 @@
       <c r="H2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="10" t="s">
         <v>37</v>
       </c>
       <c r="J2" s="1" t="b">
@@ -809,7 +815,7 @@
         <v>-2.1</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>35</v>
       </c>
@@ -835,7 +841,7 @@
       <c r="H3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I3" s="9"/>
+      <c r="I3" s="10"/>
       <c r="J3" s="1" t="b">
         <v>1</v>
       </c>
@@ -891,7 +897,7 @@
         <v>-1.7</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>36</v>
       </c>
@@ -911,13 +917,13 @@
         <v>33</v>
       </c>
       <c r="G4" s="1" t="str">
-        <f t="shared" ref="G4:G10" si="0">_xlfn.CONCAT(SUBSTITUTE(D4,".","_"),"__",A4)</f>
+        <f t="shared" ref="G4:G13" si="0">_xlfn.CONCAT(SUBSTITUTE(D4,".","_"),"__",A4)</f>
         <v>BJ_1__AZD8895</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="9"/>
+      <c r="I4" s="10"/>
       <c r="J4" s="1" t="b">
         <v>1</v>
       </c>
@@ -973,7 +979,7 @@
         <v>-2.4</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>34</v>
       </c>
@@ -999,7 +1005,7 @@
       <c r="H5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="9"/>
+      <c r="I5" s="10"/>
       <c r="J5" s="1" t="b">
         <v>1</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
@@ -1081,7 +1087,7 @@
       <c r="H6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="10"/>
       <c r="J6" s="1" t="b">
         <v>1</v>
       </c>
@@ -1137,7 +1143,7 @@
         <v>-2.1</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
@@ -1163,7 +1169,7 @@
       <c r="H7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="9"/>
+      <c r="I7" s="10"/>
       <c r="J7" s="1" t="b">
         <v>1</v>
       </c>
@@ -1219,7 +1225,7 @@
         <v>-1.9</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
@@ -1245,7 +1251,7 @@
       <c r="H8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="10"/>
       <c r="J8" s="1" t="b">
         <v>1</v>
       </c>
@@ -1301,7 +1307,7 @@
         <v>-1.1000000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
@@ -1327,7 +1333,7 @@
       <c r="H9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="10"/>
       <c r="J9" s="1" t="b">
         <v>1</v>
       </c>
@@ -1383,7 +1389,7 @@
         <v>-1.1000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
@@ -1409,7 +1415,7 @@
       <c r="H10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="9"/>
+      <c r="I10" s="10"/>
       <c r="J10" s="1" t="b">
         <v>1</v>
       </c>
@@ -1463,11 +1469,104 @@
       </c>
       <c r="AA10" s="1">
         <v>-1.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="48" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>XBB_1_5_DJM__LY-CoV1404</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="64" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>XBB_1_5_DJM__AZD1061</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>XBB_1_5_DJM__AZD8895</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="10"/>
+      <c r="J13" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I2:I10"/>
+    <mergeCell ref="I2:I13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>